<commit_message>
docs: update data schema
</commit_message>
<xml_diff>
--- a/Data_Schema.xlsx
+++ b/Data_Schema.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$C$57</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$C$58</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
   <si>
     <t>Columnas</t>
   </si>
@@ -33,15 +33,54 @@
     <t>Identificador Unico Universal (UUID) usado para identificar cada caso.</t>
   </si>
   <si>
+    <t>Me identifico (género)</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Genero autopercibido del encuestado.</t>
+  </si>
+  <si>
+    <t>Tengo (edad)</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Edad del encuestado.</t>
+  </si>
+  <si>
     <t>Dónde estás trabajando</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>Provincia desde la cuál el encuestado está trabajando. Por ejemplo: Catamarca, Chubut, La Rioja, etc.</t>
   </si>
   <si>
+    <t>Años de experiencia</t>
+  </si>
+  <si>
+    <t>String (Si bien todos son números, algunos usuarios aclaran cuando han trabajado más de 10 años por ejemplo, con +10)</t>
+  </si>
+  <si>
+    <t>Indica la cantidad de años que el encuestado lleva desempeñandose en dicho rol.</t>
+  </si>
+  <si>
+    <t>Años en el puesto actual</t>
+  </si>
+  <si>
+    <t>Float (Varios encuestados respondieron con decimales incluidos, y otros sólo con el entero)</t>
+  </si>
+  <si>
+    <t>Indicador para cuántos años lleva el encuestado trabajando en el puesto actual.</t>
+  </si>
+  <si>
+    <t>Trabajo de</t>
+  </si>
+  <si>
+    <t>Indica el trabajo que el encuestado realiza. Por ejemplo: Developer, SysAdmin / DevOps / SRE, etc.</t>
+  </si>
+  <si>
     <t>Tipo de contrato</t>
   </si>
   <si>
@@ -51,9 +90,6 @@
     <t>Salario mensual (en tu moneda local)</t>
   </si>
   <si>
-    <t>Integer</t>
-  </si>
-  <si>
     <t>Integer que indique el salario bruto del encuestado en pesos argentinos.</t>
   </si>
   <si>
@@ -105,9 +141,6 @@
     <t>¿De qué % fue el ajuste total?</t>
   </si>
   <si>
-    <t>Float (Varios encuestados respondieron con decimales incluidos, y otros sólo con el entero)</t>
-  </si>
-  <si>
     <t>El encuestado indica de qué porcentaje fue el ajuste total.</t>
   </si>
   <si>
@@ -120,21 +153,6 @@
     <t>Número que indica en qué mes el encuestado recibió el último ajuste salarial.</t>
   </si>
   <si>
-    <t>Trabajo de</t>
-  </si>
-  <si>
-    <t>Indica el trabajo que el encuestado realiza. Por ejemplo: Developer, SysAdmin / DevOps / SRE, etc.</t>
-  </si>
-  <si>
-    <t>Años de experiencia</t>
-  </si>
-  <si>
-    <t>String (Si bien todos son números, algunos usuarios aclaran cuando han trabajado más de 10 años por ejemplo, con +10)</t>
-  </si>
-  <si>
-    <t>Indica la cantidad de años que el encuestado lleva desempeñandose en dicho rol.</t>
-  </si>
-  <si>
     <t>Años en la empresa actual</t>
   </si>
   <si>
@@ -142,12 +160,6 @@
   </si>
   <si>
     <t>Indicador de la cantidad de años que el encuestado se desempeñó en su actual empresa.</t>
-  </si>
-  <si>
-    <t>Años en el puesto actual</t>
-  </si>
-  <si>
-    <t>Indicador para cuántos años lleva el encuestado trabajando en el puesto actual.</t>
   </si>
   <si>
     <t>¿Gente a cargo?</t>
@@ -347,16 +359,10 @@
     <t>Indica el tipo de nuevo beneficio instaurado.</t>
   </si>
   <si>
-    <t>Tengo (edad)</t>
-  </si>
-  <si>
-    <t>Edad del encuestado.</t>
-  </si>
-  <si>
-    <t>Me identifico (género)</t>
-  </si>
-  <si>
-    <t>Genero autopercibido del encuestado.</t>
+    <t>Valor dólar informal semestral</t>
+  </si>
+  <si>
+    <t>Valor del dolar informal (blue) para ese semestre.</t>
   </si>
 </sst>
 </file>
@@ -709,18 +715,18 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>13</v>
@@ -731,95 +737,95 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>34</v>
@@ -841,51 +847,51 @@
         <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>48</v>
@@ -896,7 +902,7 @@
         <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>50</v>
@@ -984,7 +990,7 @@
         <v>65</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>66</v>
@@ -1006,7 +1012,7 @@
         <v>69</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>70</v>
@@ -1028,7 +1034,7 @@
         <v>73</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>74</v>
@@ -1097,172 +1103,172 @@
         <v>7</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55">
@@ -1270,7 +1276,7 @@
         <v>108</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>109</v>
@@ -1281,7 +1287,7 @@
         <v>110</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>111</v>
@@ -1298,8 +1304,19 @@
         <v>113</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$C$57"/>
+  <autoFilter ref="$A$1:$C$58"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>